<commit_message>
no question embedding, evaluation
</commit_message>
<xml_diff>
--- a/static_data/QA_Race.xlsx
+++ b/static_data/QA_Race.xlsx
@@ -14394,7 +14394,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14404,13 +14404,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -14508,7 +14502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14522,7 +14516,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -14531,17 +14528,17 @@
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14855,7 +14852,7 @@
   <cols>
     <col min="1" max="1" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="11" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="67.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="67.29071428571429" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="11" width="15.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="11" width="39.005" customWidth="1" bestFit="1"/>
@@ -14885,7 +14882,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="51.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="58.5">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -14908,7 +14905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="51.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="58.5">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -14931,7 +14928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="51.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="58.5">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -14954,7 +14951,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="39.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="45.75">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -14977,7 +14974,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="39.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="45.75">
       <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
@@ -15000,7 +14997,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="39.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="45.75">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>